<commit_message>
change check_combination to line
</commit_message>
<xml_diff>
--- a/back/modsandbox/test_data/rule1.xlsx
+++ b/back/modsandbox/test_data/rule1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/woogler/dev/reddit_virtual_sandbox/back/modsandbox/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0D5AC138-6F13-6A41-8D37-BD42C21085E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65BCC63-9CDF-4943-9BFB-80CE084FFC61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20180" yWindow="13380" windowWidth="27900" windowHeight="16940"/>
+    <workbookView xWindow="880" yWindow="500" windowWidth="27900" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rule1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="90">
   <si>
     <t>id</t>
   </si>
@@ -113,14 +113,6 @@
     <t>Looking to make a career change; hoping to get some input</t>
   </si>
   <si>
-    <t>For some background, I've been working around 5 years in corporate healthcare IT (very much customer facing; not really any coding/programming experience required at all). I've been feeling very much like I needed to go elsewhere for a while but I haven't had a good push as the job pays OK and offers great benefits (but with 0 upward mobility).
-However, last week I had a medical incident and at this point I'm not sure if I'll be able to safely drive as much (if at all), even going up and down stairs can be a challenge. I'm on medical leave from work while waiting on specialists and referrals etc. but I'm coming from an IT job that involved a large amount of walking. And work from home would be challenging as we already have a help desk that handles most remote issues (management already decided to not let people WFH as there was fear of just downsizing and outsourcing everyone).
-I realized that it'd be much better for me in the long term to switch to a career that allows more work from home/flexibility and could hopefully offer much better pay - right now with my current job I don't see myself having a long term career/retirement plan, and until I hear from my doctors I'm stuck on medical leave wondering if I'll even be able to go back to my job.
-I've been looking into coding bootcamps (as I'd rather not spend 4 years in school racking up tons of debt), but a lot seem really sketchy. The one I see most advertised/recommended is App Authority, but there's literally no way to schedule a talk with admissions (which seems really suspicious). They claim you pay nothing upfront until you "find a job" making $50k+, but they don't specify that it's a software engineer job. My current job I make a little over $50k, so it would be nice to avoid paying large sums while at a job I may or may not be able to go back to at all.
-&amp;#x200B;
-**TL;DR** I'm in my late 30s, may or may not be disabled/unable to walk/drive reliably, and want to break into software engineering/half-stack/full-stack. Where the heck do I start? Have a small amount of experience with C++/Python but nothing serious. TIA</t>
-  </si>
-  <si>
     <t>n5tfwx</t>
   </si>
   <si>
@@ -209,12 +201,6 @@
   </si>
   <si>
     <t>Is total career change at 30 possible?</t>
-  </si>
-  <si>
-    <t>I am currently a 29 year old male living in southern europe. A have a Bsc in business management and have  worked for the past 4 years in digital marketing. In September I left my job because it was really hard for me to keep doing it as I knew I could never do it for the rest of my life. I spend most of my time till today trying to find out what I would like to do and I think I have a clue. 
-I always like data and playing with excel or similar programs. I think data science and machine learning are very interesting and would like to get involved in that. As you probably understand I have very limited code knowledge as the only connection is creating scripts in autohotkey. I do not know any programming languages but I learn quickly and I am really interested in programming. 
-Do you think I have a chance in ever advancing in machine learning or data science? Is it even possible to get a job in a position like this at this age with zero knowledge? 
-PS. I am determined to study a lot and if anyone has advice of how to better proceed it would be really appreciated.</t>
   </si>
   <si>
     <t>n4qi4o</t>
@@ -371,14 +357,46 @@
 Here's my question. I still really like programming, and I would really like to pursue a career in the area after college, or even during it. But is that a realistic goal if I'm just getting a major in philosophy? I know I could go back to college, but at this point, I really don't see that happening.</t>
   </si>
   <si>
-    <t>criteria</t>
+    <t>minor</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>I am currently a 29 year old male living in southern europe. A have a Bsc in business management and have  worked for the past 4 years in digital marketing. In September I left my job because it was really hard for me to keep doing it as I knew I could never do it for the rest of my life. I spend most of my time till today trying to find out what I would like to do and I think I have a clue. 
+I always like data and playing with excel or similar programs. I think data science and machine learning are very interesting and would like to get involved in that. As you probably understand I have very limited code knowledge as the only connection is creating scripts in autohotkey. I do not know any programming languages but I learn quickly and I am really interested in programming. 
+Do you think I have a chance in ever advancing in machine learning or data science? Is it even possible to get a job in a position like this at this age with zero knowledge? 
+PS. I am determined to study a lot and if anyone has advice of how to better proceed it would be really appreciated.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ML/DS</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>internship</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>no mention degree</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bootcamp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>For some background, I've been working around 5 years in corporate healthcare IT (very much customer facing; not really any coding/programming experience required at all). I've been feeling very much like I needed to go elsewhere for a while but I haven't had a good push as the job pays OK and offers great benefits (but with 0 upward mobility).
+However, last week I had a medical incident and at this point I'm not sure if I'll be able to safely drive as much (if at all), even going up and down stairs can be a challenge. I'm on medical leave from work while waiting on specialists and referrals etc. but I'm coming from an IT job that involved a large amount of walking. And work from home would be challenging as we already have a help desk that handles most remote issues (management already decided to not let people WFH as there was fear of just downsizing and outsourcing everyone).
+I realized that it'd be much better for me in the long term to switch to a career that allows more work from home/flexibility and could hopefully offer much better pay - right now with my current job I don't see myself having a long term career/retirement plan, and until I hear from my doctors I'm stuck on medical leave wondering if I'll even be able to go back to my job.
+I've been looking into coding bootcamps (as I'd rather not spend 4 years in school racking up tons of debt), but a lot seem really sketchy. The one I see most advertised/recommended is App Authority, but there's literally no way to schedule a talk with admissions (which seems really suspicious). They claim you pay nothing upfront until you "find a job" making $50k+, but they don't specify that it's a software engineer job. My current job I make a little over $50k, so it would be nice to avoid paying large sums while at a job I may or may not be able to go back to at all.
+&amp;#x200B;
+**TL;DR** I'm in my late 30s, may or may not be disabled/unable to walk/drive reliably, and want to break into software engineering/half-stack/full-stack. Where the heck do I start? Have a small amount of experience with C++/Python but nothing serious. TIA</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19">
     <font>
       <sz val="12"/>
@@ -1326,20 +1344,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
     <col min="4" max="4" width="78.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:9">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1350,10 +1371,22 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="409.6">
+      <c r="G1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="171">
       <c r="A2">
         <v>40</v>
       </c>
@@ -1367,7 +1400,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="409.6">
+    <row r="3" spans="1:9" ht="171">
       <c r="A3">
         <v>101</v>
       </c>
@@ -1381,7 +1414,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="409.6">
+    <row r="4" spans="1:9" ht="304">
       <c r="A4">
         <v>137</v>
       </c>
@@ -1394,8 +1427,11 @@
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="409.6">
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="409.6">
       <c r="A5">
         <v>148</v>
       </c>
@@ -1409,7 +1445,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="409.6">
+    <row r="6" spans="1:9" ht="304">
       <c r="A6">
         <v>159</v>
       </c>
@@ -1422,8 +1458,11 @@
       <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="409.6">
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="323">
       <c r="A7">
         <v>183</v>
       </c>
@@ -1437,7 +1476,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="409.6">
+    <row r="8" spans="1:9" ht="409.6">
       <c r="A8">
         <v>196</v>
       </c>
@@ -1448,305 +1487,330 @@
         <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="409.6">
+        <v>89</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="380">
       <c r="A9">
         <v>209</v>
       </c>
       <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
         <v>24</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="409.6">
+    </row>
+    <row r="10" spans="1:9" ht="266">
       <c r="A10">
         <v>217</v>
       </c>
       <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
         <v>27</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="409.6">
+    </row>
+    <row r="11" spans="1:9" ht="114">
       <c r="A11">
         <v>229</v>
       </c>
       <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
         <v>30</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="409.6">
+    </row>
+    <row r="12" spans="1:9" ht="152">
       <c r="A12">
         <v>245</v>
       </c>
       <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
         <v>33</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="409.6">
+    </row>
+    <row r="13" spans="1:9" ht="171">
       <c r="A13">
         <v>258</v>
       </c>
       <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
         <v>36</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="409.6">
+      <c r="I13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="409.6">
       <c r="A14">
         <v>259</v>
       </c>
       <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
         <v>39</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="409.6">
+    </row>
+    <row r="15" spans="1:9" ht="409.6">
       <c r="A15">
         <v>260</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>261</v>
       </c>
       <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
         <v>43</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>44</v>
       </c>
-      <c r="D16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="409.6">
+    </row>
+    <row r="17" spans="1:9" ht="285">
       <c r="A17">
         <v>281</v>
       </c>
       <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
         <v>46</v>
       </c>
-      <c r="C17" t="s">
-        <v>47</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="409.6">
+        <v>84</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="409.6">
       <c r="A18">
         <v>346</v>
       </c>
       <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="409.6">
+    </row>
+    <row r="19" spans="1:9" ht="171">
       <c r="A19">
         <v>364</v>
       </c>
       <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>366</v>
       </c>
       <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" t="s">
         <v>55</v>
       </c>
-      <c r="C20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="409.6">
+    </row>
+    <row r="21" spans="1:9" ht="323">
       <c r="A21">
         <v>387</v>
       </c>
       <c r="B21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="409.6">
+      <c r="I21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="95">
       <c r="A22">
         <v>403</v>
       </c>
       <c r="B22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="409.6">
+    </row>
+    <row r="23" spans="1:9" ht="409.6">
       <c r="A23">
         <v>433</v>
       </c>
       <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C23" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="409.6">
+    </row>
+    <row r="24" spans="1:9" ht="409.6">
       <c r="A24">
         <v>434</v>
       </c>
       <c r="B24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C24" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="409.6">
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="304">
       <c r="A25">
         <v>449</v>
       </c>
       <c r="B25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C25" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="409.6">
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="285">
       <c r="A26">
         <v>451</v>
       </c>
       <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C26" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="409.6">
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="409.6">
       <c r="A27">
         <v>455</v>
       </c>
       <c r="B27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C27" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>459</v>
       </c>
       <c r="B28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" t="s">
         <v>79</v>
       </c>
-      <c r="C28" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="409.6">
+    </row>
+    <row r="29" spans="1:9" ht="247">
       <c r="A29">
         <v>529</v>
       </c>
       <c r="B29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C29" t="s">
-        <v>83</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>